<commit_message>
Work on line graph
</commit_message>
<xml_diff>
--- a/results/averagePrecisions.xlsx
+++ b/results/averagePrecisions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\v-riaktu\IdeaProjects\graph2vec\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E4AC08A-C0A4-413A-B0AE-AD21FBB95FE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A70757B-CA79-4957-B45C-A059EEB07899}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="25">
   <si>
     <t>dataset</t>
   </si>
@@ -92,6 +92,9 @@
   </si>
   <si>
     <t>TGSM</t>
+  </si>
+  <si>
+    <t>Line Graph:</t>
   </si>
 </sst>
 </file>
@@ -575,9 +578,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -774,8 +778,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:L37" totalsRowShown="0">
-  <autoFilter ref="A1:L37" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:L38" totalsRowShown="0">
+  <autoFilter ref="A1:L38" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="dataset"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="embedding_method"/>
@@ -1091,10 +1095,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L37"/>
+  <dimension ref="A1:L63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G69" sqref="G69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2518,11 +2522,967 @@
         <v>0</v>
       </c>
     </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A38" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A39" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K39" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L39" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A40" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D40" s="1">
+        <v>0.44</v>
+      </c>
+      <c r="E40" s="1">
+        <v>0.44</v>
+      </c>
+      <c r="F40" s="1">
+        <v>0.44</v>
+      </c>
+      <c r="G40" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="H40" s="1">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="I40" s="1">
+        <v>0.63</v>
+      </c>
+      <c r="J40" s="1">
+        <v>0.44</v>
+      </c>
+      <c r="K40" s="1">
+        <v>0.44</v>
+      </c>
+      <c r="L40" s="1">
+        <v>0.44</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A41" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D41" s="1">
+        <v>0.45</v>
+      </c>
+      <c r="E41" s="1">
+        <v>0.35</v>
+      </c>
+      <c r="F41" s="1">
+        <v>0.46</v>
+      </c>
+      <c r="G41" s="1">
+        <v>0</v>
+      </c>
+      <c r="H41" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="I41" s="1">
+        <v>0.32</v>
+      </c>
+      <c r="J41" s="1">
+        <v>0.43</v>
+      </c>
+      <c r="K41" s="1">
+        <v>0.46</v>
+      </c>
+      <c r="L41" s="1">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A42" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D42" s="1">
+        <v>0.27</v>
+      </c>
+      <c r="E42" s="1">
+        <v>0.21</v>
+      </c>
+      <c r="F42" s="1">
+        <v>0.32</v>
+      </c>
+      <c r="G42" s="1">
+        <v>0</v>
+      </c>
+      <c r="H42" s="1">
+        <v>0.23</v>
+      </c>
+      <c r="I42" s="1">
+        <v>0.23</v>
+      </c>
+      <c r="J42" s="1">
+        <v>0.21</v>
+      </c>
+      <c r="K42" s="1">
+        <v>0.32</v>
+      </c>
+      <c r="L42" s="1">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A43" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D43" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="E43" s="1">
+        <v>0.24</v>
+      </c>
+      <c r="F43" s="1">
+        <v>0.21</v>
+      </c>
+      <c r="G43" s="1">
+        <v>0</v>
+      </c>
+      <c r="H43" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="I43" s="1">
+        <v>0.22</v>
+      </c>
+      <c r="J43" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="K43" s="1">
+        <v>0.21</v>
+      </c>
+      <c r="L43" s="1">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A44" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D44" s="1">
+        <v>0.22</v>
+      </c>
+      <c r="E44" s="1">
+        <v>0.21</v>
+      </c>
+      <c r="F44" s="1">
+        <v>0.23</v>
+      </c>
+      <c r="G44" s="1">
+        <v>0</v>
+      </c>
+      <c r="H44" s="1">
+        <v>0.23</v>
+      </c>
+      <c r="I44" s="1">
+        <v>0.22</v>
+      </c>
+      <c r="J44" s="1">
+        <v>0.22</v>
+      </c>
+      <c r="K44" s="1">
+        <v>0.23</v>
+      </c>
+      <c r="L44" s="1">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A45" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D45" s="1">
+        <v>0.24</v>
+      </c>
+      <c r="E45" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="F45" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="G45" s="1">
+        <v>0</v>
+      </c>
+      <c r="H45" s="1">
+        <v>0.27</v>
+      </c>
+      <c r="I45" s="1">
+        <v>0.23</v>
+      </c>
+      <c r="J45" s="1">
+        <v>0.24</v>
+      </c>
+      <c r="K45" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="L45" s="1">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A46" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D46" s="1">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="E46" s="1">
+        <v>0.39</v>
+      </c>
+      <c r="F46" s="1">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="G46" s="1">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="H46" s="1">
+        <v>0.26</v>
+      </c>
+      <c r="I46" s="1">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="J46" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="K46" s="1">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="L46" s="1">
+        <v>0.39</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A47" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D47" s="1">
+        <v>0.26</v>
+      </c>
+      <c r="E47" s="1">
+        <v>0.46</v>
+      </c>
+      <c r="F47" s="1">
+        <v>0.27</v>
+      </c>
+      <c r="G47" s="1">
+        <v>0</v>
+      </c>
+      <c r="H47" s="1">
+        <v>0.23</v>
+      </c>
+      <c r="I47" s="1">
+        <v>0.22</v>
+      </c>
+      <c r="J47" s="1">
+        <v>0.22</v>
+      </c>
+      <c r="K47" s="1">
+        <v>0.27</v>
+      </c>
+      <c r="L47" s="1">
+        <v>0.46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A48" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D48" s="1">
+        <v>0.36</v>
+      </c>
+      <c r="E48" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="F48" s="1">
+        <v>0.37</v>
+      </c>
+      <c r="G48" s="1">
+        <v>0</v>
+      </c>
+      <c r="H48" s="1">
+        <v>0.22</v>
+      </c>
+      <c r="I48" s="1">
+        <v>0.22</v>
+      </c>
+      <c r="J48" s="1">
+        <v>0.36</v>
+      </c>
+      <c r="K48" s="1">
+        <v>0.37</v>
+      </c>
+      <c r="L48" s="1">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A49" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D49" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="E49" s="1">
+        <v>0.21</v>
+      </c>
+      <c r="F49" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="G49" s="1">
+        <v>0</v>
+      </c>
+      <c r="H49" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="I49" s="1">
+        <v>0.21</v>
+      </c>
+      <c r="J49" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="K49" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="L49" s="1">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A50" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D50" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="E50" s="1">
+        <v>0.26</v>
+      </c>
+      <c r="F50" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="G50" s="1">
+        <v>0</v>
+      </c>
+      <c r="H50" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="I50" s="1">
+        <v>0.24</v>
+      </c>
+      <c r="J50" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="K50" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="L50" s="1">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A51" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D51" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="E51" s="1">
+        <v>0.26</v>
+      </c>
+      <c r="F51" s="1">
+        <v>0.26</v>
+      </c>
+      <c r="G51" s="1">
+        <v>0</v>
+      </c>
+      <c r="H51" s="1">
+        <v>0.27</v>
+      </c>
+      <c r="I51" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="J51" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="K51" s="1">
+        <v>0.26</v>
+      </c>
+      <c r="L51" s="1">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A52" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D52" s="1">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E52" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="F52" s="1">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G52" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="H52" s="1">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="I52" s="1">
+        <v>0.08</v>
+      </c>
+      <c r="J52" s="1">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="K52" s="1">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="L52" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A53" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D53" s="1">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E53" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="F53" s="1">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G53" s="1">
+        <v>0</v>
+      </c>
+      <c r="H53" s="1">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="I53" s="1">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="J53" s="1">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="K53" s="1">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="L53" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A54" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D54" s="1">
+        <v>0</v>
+      </c>
+      <c r="E54" s="1">
+        <v>0</v>
+      </c>
+      <c r="F54" s="1">
+        <v>0</v>
+      </c>
+      <c r="G54" s="1">
+        <v>0</v>
+      </c>
+      <c r="H54" s="1">
+        <v>0</v>
+      </c>
+      <c r="I54" s="1">
+        <v>0</v>
+      </c>
+      <c r="J54" s="1">
+        <v>0</v>
+      </c>
+      <c r="K54" s="1">
+        <v>0</v>
+      </c>
+      <c r="L54" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A55" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D55" s="1">
+        <v>0</v>
+      </c>
+      <c r="E55" s="1">
+        <v>0</v>
+      </c>
+      <c r="F55" s="1">
+        <v>0</v>
+      </c>
+      <c r="G55" s="1">
+        <v>0</v>
+      </c>
+      <c r="H55" s="1">
+        <v>0</v>
+      </c>
+      <c r="I55" s="1">
+        <v>0</v>
+      </c>
+      <c r="J55" s="1">
+        <v>0</v>
+      </c>
+      <c r="K55" s="1">
+        <v>0</v>
+      </c>
+      <c r="L55" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A56" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D56" s="1">
+        <v>0</v>
+      </c>
+      <c r="E56" s="1">
+        <v>0</v>
+      </c>
+      <c r="F56" s="1">
+        <v>0</v>
+      </c>
+      <c r="G56" s="1">
+        <v>0</v>
+      </c>
+      <c r="H56" s="1">
+        <v>0</v>
+      </c>
+      <c r="I56" s="1">
+        <v>0</v>
+      </c>
+      <c r="J56" s="1">
+        <v>0</v>
+      </c>
+      <c r="K56" s="1">
+        <v>0</v>
+      </c>
+      <c r="L56" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A57" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D57" s="1">
+        <v>0</v>
+      </c>
+      <c r="E57" s="1">
+        <v>0</v>
+      </c>
+      <c r="F57" s="1">
+        <v>0</v>
+      </c>
+      <c r="G57" s="1">
+        <v>0</v>
+      </c>
+      <c r="H57" s="1">
+        <v>0</v>
+      </c>
+      <c r="I57" s="1">
+        <v>0</v>
+      </c>
+      <c r="J57" s="1">
+        <v>0</v>
+      </c>
+      <c r="K57" s="1">
+        <v>0</v>
+      </c>
+      <c r="L57" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A58" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D58" s="1">
+        <v>0.42</v>
+      </c>
+      <c r="E58" s="1">
+        <v>0.42</v>
+      </c>
+      <c r="F58" s="1">
+        <v>0.38</v>
+      </c>
+      <c r="G58" s="1">
+        <v>0.67</v>
+      </c>
+      <c r="H58" s="1">
+        <v>0.48</v>
+      </c>
+      <c r="I58" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="J58" s="1">
+        <v>0.63</v>
+      </c>
+      <c r="K58" s="1">
+        <v>0.38</v>
+      </c>
+      <c r="L58" s="1">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A59" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D59" s="1">
+        <v>0.44</v>
+      </c>
+      <c r="E59" s="1">
+        <v>0.45</v>
+      </c>
+      <c r="F59" s="1">
+        <v>0.44</v>
+      </c>
+      <c r="G59" s="1">
+        <v>0</v>
+      </c>
+      <c r="H59" s="1">
+        <v>0.48</v>
+      </c>
+      <c r="I59" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="J59" s="1">
+        <v>0.44</v>
+      </c>
+      <c r="K59" s="1">
+        <v>0.44</v>
+      </c>
+      <c r="L59" s="1">
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A60" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D60" s="1">
+        <v>0.48</v>
+      </c>
+      <c r="E60" s="1">
+        <v>0.45</v>
+      </c>
+      <c r="F60" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="G60" s="1">
+        <v>0</v>
+      </c>
+      <c r="H60" s="1">
+        <v>0.48</v>
+      </c>
+      <c r="I60" s="1">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="J60" s="1">
+        <v>0.48</v>
+      </c>
+      <c r="K60" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="L60" s="1">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A61" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D61" s="1">
+        <v>0.59</v>
+      </c>
+      <c r="E61" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="F61" s="1">
+        <v>0.59</v>
+      </c>
+      <c r="G61" s="1">
+        <v>0</v>
+      </c>
+      <c r="H61" s="1">
+        <v>0.59</v>
+      </c>
+      <c r="I61" s="1">
+        <v>0.52</v>
+      </c>
+      <c r="J61" s="1">
+        <v>0.59</v>
+      </c>
+      <c r="K61" s="1">
+        <v>0.59</v>
+      </c>
+      <c r="L61" s="1">
+        <v>0.51</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A62" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D62" s="1">
+        <v>0.54</v>
+      </c>
+      <c r="E62" s="1">
+        <v>0.63</v>
+      </c>
+      <c r="F62" s="1">
+        <v>0.54</v>
+      </c>
+      <c r="G62" s="1">
+        <v>0</v>
+      </c>
+      <c r="H62" s="1">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="I62" s="1">
+        <v>0.49</v>
+      </c>
+      <c r="J62" s="1">
+        <v>0.49</v>
+      </c>
+      <c r="K62" s="1">
+        <v>0.54</v>
+      </c>
+      <c r="L62" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A63" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D63" s="1">
+        <v>0.54</v>
+      </c>
+      <c r="E63" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="F63" s="1">
+        <v>0.54</v>
+      </c>
+      <c r="G63" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="H63" s="1">
+        <v>0.54</v>
+      </c>
+      <c r="I63" s="1">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="J63" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="K63" s="1">
+        <v>0.54</v>
+      </c>
+      <c r="L63" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
TGSM and BBR graph2vec results are added
</commit_message>
<xml_diff>
--- a/results/averagePrecisions.xlsx
+++ b/results/averagePrecisions.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\v-riaktu\IdeaProjects\graph2vec\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A70757B-CA79-4957-B45C-A059EEB07899}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A15C0E6-E61D-4B42-8E1F-123EE857EB9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="26">
   <si>
     <t>dataset</t>
   </si>
@@ -95,6 +95,9 @@
   </si>
   <si>
     <t>Line Graph:</t>
+  </si>
+  <si>
+    <t>BBR</t>
   </si>
 </sst>
 </file>
@@ -578,10 +581,14 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -778,8 +785,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:L38" totalsRowShown="0">
-  <autoFilter ref="A1:L38" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:L39" totalsRowShown="0">
+  <autoFilter ref="A1:L39" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="dataset"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="embedding_method"/>
@@ -1095,10 +1102,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L63"/>
+  <dimension ref="A1:L66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="G69" sqref="G69"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C68" sqref="C68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2456,32 +2463,32 @@
       <c r="C36" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D36" s="1">
-        <v>0</v>
-      </c>
-      <c r="E36" s="1">
-        <v>0</v>
-      </c>
-      <c r="F36" s="1">
-        <v>0</v>
-      </c>
-      <c r="G36" s="1">
-        <v>0</v>
-      </c>
-      <c r="H36" s="1">
-        <v>0</v>
-      </c>
-      <c r="I36" s="1">
-        <v>0</v>
-      </c>
-      <c r="J36" s="1">
-        <v>0</v>
-      </c>
-      <c r="K36" s="1">
-        <v>0</v>
-      </c>
-      <c r="L36" s="1">
-        <v>0</v>
+      <c r="D36" s="4">
+        <v>0.59</v>
+      </c>
+      <c r="E36" s="4">
+        <v>0.45</v>
+      </c>
+      <c r="F36" s="4">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="G36" s="4">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="H36" s="4">
+        <v>0.53</v>
+      </c>
+      <c r="I36" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="J36" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="K36" s="4">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="L36" s="4">
+        <v>0.5</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.35">
@@ -2494,189 +2501,151 @@
       <c r="C37" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D37" s="1">
-        <v>0</v>
-      </c>
-      <c r="E37" s="1">
-        <v>0</v>
-      </c>
-      <c r="F37" s="1">
-        <v>0</v>
-      </c>
-      <c r="G37" s="1">
-        <v>0</v>
-      </c>
-      <c r="H37" s="1">
-        <v>0</v>
-      </c>
-      <c r="I37" s="1">
-        <v>0</v>
-      </c>
-      <c r="J37" s="1">
-        <v>0</v>
-      </c>
-      <c r="K37" s="1">
-        <v>0</v>
-      </c>
-      <c r="L37" s="1">
-        <v>0</v>
+      <c r="D37" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="E37" s="3">
+        <v>0.47</v>
+      </c>
+      <c r="F37" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="G37" s="3">
+        <v>0</v>
+      </c>
+      <c r="H37" s="3">
+        <v>0.51</v>
+      </c>
+      <c r="I37" s="3">
+        <v>0.43</v>
+      </c>
+      <c r="J37" s="3">
+        <v>0.48</v>
+      </c>
+      <c r="K37" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="L37" s="3">
+        <v>0.42</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A38" s="2" t="s">
+      <c r="A38" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D38" s="6">
+        <v>0.08</v>
+      </c>
+      <c r="E38" s="6">
+        <v>0.05</v>
+      </c>
+      <c r="F38" s="6">
+        <v>0.08</v>
+      </c>
+      <c r="G38" s="6">
+        <v>0.04</v>
+      </c>
+      <c r="H38" s="6">
+        <v>0.08</v>
+      </c>
+      <c r="I38" s="6">
+        <v>0.08</v>
+      </c>
+      <c r="J38" s="6">
+        <v>0.12</v>
+      </c>
+      <c r="K38" s="6">
+        <v>0.08</v>
+      </c>
+      <c r="L38" s="6">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A39" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D39" s="5">
+        <v>0.06</v>
+      </c>
+      <c r="E39" s="5">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="F39" s="5">
+        <v>0.06</v>
+      </c>
+      <c r="G39" s="5">
+        <v>0</v>
+      </c>
+      <c r="H39" s="5">
+        <v>0.06</v>
+      </c>
+      <c r="I39" s="5">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="J39" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="K39" s="5">
+        <v>0.06</v>
+      </c>
+      <c r="L39" s="5">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A41" s="2" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A39" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G39" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H39" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I39" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J39" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K39" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L39" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A40" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D40" s="1">
-        <v>0.44</v>
-      </c>
-      <c r="E40" s="1">
-        <v>0.44</v>
-      </c>
-      <c r="F40" s="1">
-        <v>0.44</v>
-      </c>
-      <c r="G40" s="1">
-        <v>0.25</v>
-      </c>
-      <c r="H40" s="1">
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="I40" s="1">
-        <v>0.63</v>
-      </c>
-      <c r="J40" s="1">
-        <v>0.44</v>
-      </c>
-      <c r="K40" s="1">
-        <v>0.44</v>
-      </c>
-      <c r="L40" s="1">
-        <v>0.44</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A41" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D41" s="1">
-        <v>0.45</v>
-      </c>
-      <c r="E41" s="1">
-        <v>0.35</v>
-      </c>
-      <c r="F41" s="1">
-        <v>0.46</v>
-      </c>
-      <c r="G41" s="1">
-        <v>0</v>
-      </c>
-      <c r="H41" s="1">
-        <v>0.3</v>
-      </c>
-      <c r="I41" s="1">
-        <v>0.32</v>
-      </c>
-      <c r="J41" s="1">
-        <v>0.43</v>
-      </c>
-      <c r="K41" s="1">
-        <v>0.46</v>
-      </c>
-      <c r="L41" s="1">
-        <v>0.35</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D42" s="1">
-        <v>0.27</v>
-      </c>
-      <c r="E42" s="1">
-        <v>0.21</v>
-      </c>
-      <c r="F42" s="1">
-        <v>0.32</v>
-      </c>
-      <c r="G42" s="1">
-        <v>0</v>
-      </c>
-      <c r="H42" s="1">
-        <v>0.23</v>
-      </c>
-      <c r="I42" s="1">
-        <v>0.23</v>
-      </c>
-      <c r="J42" s="1">
-        <v>0.21</v>
-      </c>
-      <c r="K42" s="1">
-        <v>0.32</v>
-      </c>
-      <c r="L42" s="1">
-        <v>0.21</v>
+        <v>2</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J42" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K42" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L42" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.35">
@@ -2684,37 +2653,37 @@
         <v>12</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D43" s="1">
-        <v>0.2</v>
+        <v>0.44</v>
       </c>
       <c r="E43" s="1">
-        <v>0.24</v>
+        <v>0.44</v>
       </c>
       <c r="F43" s="1">
-        <v>0.21</v>
+        <v>0.44</v>
       </c>
       <c r="G43" s="1">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="H43" s="1">
-        <v>0.2</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="I43" s="1">
-        <v>0.22</v>
+        <v>0.63</v>
       </c>
       <c r="J43" s="1">
-        <v>0.2</v>
+        <v>0.44</v>
       </c>
       <c r="K43" s="1">
-        <v>0.21</v>
+        <v>0.44</v>
       </c>
       <c r="L43" s="1">
-        <v>0.24</v>
+        <v>0.44</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.35">
@@ -2722,37 +2691,37 @@
         <v>12</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D44" s="1">
-        <v>0.22</v>
+        <v>0.45</v>
       </c>
       <c r="E44" s="1">
-        <v>0.21</v>
+        <v>0.35</v>
       </c>
       <c r="F44" s="1">
-        <v>0.23</v>
+        <v>0.46</v>
       </c>
       <c r="G44" s="1">
         <v>0</v>
       </c>
       <c r="H44" s="1">
-        <v>0.23</v>
+        <v>0.3</v>
       </c>
       <c r="I44" s="1">
-        <v>0.22</v>
+        <v>0.32</v>
       </c>
       <c r="J44" s="1">
-        <v>0.22</v>
+        <v>0.43</v>
       </c>
       <c r="K44" s="1">
-        <v>0.23</v>
+        <v>0.46</v>
       </c>
       <c r="L44" s="1">
-        <v>0.22</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.35">
@@ -2760,95 +2729,95 @@
         <v>12</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D45" s="1">
-        <v>0.24</v>
+        <v>0.27</v>
       </c>
       <c r="E45" s="1">
-        <v>0.25</v>
+        <v>0.21</v>
       </c>
       <c r="F45" s="1">
-        <v>0.25</v>
+        <v>0.32</v>
       </c>
       <c r="G45" s="1">
         <v>0</v>
       </c>
       <c r="H45" s="1">
-        <v>0.27</v>
+        <v>0.23</v>
       </c>
       <c r="I45" s="1">
         <v>0.23</v>
       </c>
       <c r="J45" s="1">
-        <v>0.24</v>
+        <v>0.21</v>
       </c>
       <c r="K45" s="1">
-        <v>0.25</v>
+        <v>0.32</v>
       </c>
       <c r="L45" s="1">
-        <v>0.24</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D46" s="1">
-        <v>0.28999999999999998</v>
+        <v>0.2</v>
       </c>
       <c r="E46" s="1">
-        <v>0.39</v>
+        <v>0.24</v>
       </c>
       <c r="F46" s="1">
-        <v>0.28000000000000003</v>
+        <v>0.21</v>
       </c>
       <c r="G46" s="1">
-        <v>0.28000000000000003</v>
+        <v>0</v>
       </c>
       <c r="H46" s="1">
-        <v>0.26</v>
+        <v>0.2</v>
       </c>
       <c r="I46" s="1">
-        <v>0.28000000000000003</v>
+        <v>0.22</v>
       </c>
       <c r="J46" s="1">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="K46" s="1">
-        <v>0.28000000000000003</v>
+        <v>0.21</v>
       </c>
       <c r="L46" s="1">
-        <v>0.39</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D47" s="1">
-        <v>0.26</v>
+        <v>0.22</v>
       </c>
       <c r="E47" s="1">
-        <v>0.46</v>
+        <v>0.21</v>
       </c>
       <c r="F47" s="1">
-        <v>0.27</v>
+        <v>0.23</v>
       </c>
       <c r="G47" s="1">
         <v>0</v>
@@ -2863,48 +2832,48 @@
         <v>0.22</v>
       </c>
       <c r="K47" s="1">
-        <v>0.27</v>
+        <v>0.23</v>
       </c>
       <c r="L47" s="1">
-        <v>0.46</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D48" s="1">
-        <v>0.36</v>
+        <v>0.24</v>
       </c>
       <c r="E48" s="1">
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
       <c r="F48" s="1">
-        <v>0.37</v>
+        <v>0.25</v>
       </c>
       <c r="G48" s="1">
         <v>0</v>
       </c>
       <c r="H48" s="1">
-        <v>0.22</v>
+        <v>0.27</v>
       </c>
       <c r="I48" s="1">
-        <v>0.22</v>
+        <v>0.23</v>
       </c>
       <c r="J48" s="1">
-        <v>0.36</v>
+        <v>0.24</v>
       </c>
       <c r="K48" s="1">
-        <v>0.37</v>
+        <v>0.25</v>
       </c>
       <c r="L48" s="1">
-        <v>0.21</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.35">
@@ -2912,37 +2881,37 @@
         <v>19</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D49" s="1">
-        <v>0.2</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="E49" s="1">
-        <v>0.21</v>
+        <v>0.39</v>
       </c>
       <c r="F49" s="1">
-        <v>0.2</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="G49" s="1">
-        <v>0</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="H49" s="1">
-        <v>0.2</v>
+        <v>0.26</v>
       </c>
       <c r="I49" s="1">
-        <v>0.21</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="J49" s="1">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="K49" s="1">
-        <v>0.2</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="L49" s="1">
-        <v>0.21</v>
+        <v>0.39</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.35">
@@ -2950,37 +2919,37 @@
         <v>19</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D50" s="1">
-        <v>0.25</v>
+        <v>0.26</v>
       </c>
       <c r="E50" s="1">
-        <v>0.26</v>
+        <v>0.46</v>
       </c>
       <c r="F50" s="1">
-        <v>0.25</v>
+        <v>0.27</v>
       </c>
       <c r="G50" s="1">
         <v>0</v>
       </c>
       <c r="H50" s="1">
-        <v>0.25</v>
+        <v>0.23</v>
       </c>
       <c r="I50" s="1">
-        <v>0.24</v>
+        <v>0.22</v>
       </c>
       <c r="J50" s="1">
-        <v>0.25</v>
+        <v>0.22</v>
       </c>
       <c r="K50" s="1">
-        <v>0.25</v>
+        <v>0.27</v>
       </c>
       <c r="L50" s="1">
-        <v>0.26</v>
+        <v>0.46</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.35">
@@ -2988,151 +2957,151 @@
         <v>19</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D51" s="1">
-        <v>0.25</v>
+        <v>0.36</v>
       </c>
       <c r="E51" s="1">
-        <v>0.26</v>
+        <v>0.2</v>
       </c>
       <c r="F51" s="1">
-        <v>0.26</v>
+        <v>0.37</v>
       </c>
       <c r="G51" s="1">
         <v>0</v>
       </c>
       <c r="H51" s="1">
-        <v>0.27</v>
+        <v>0.22</v>
       </c>
       <c r="I51" s="1">
-        <v>0.25</v>
+        <v>0.22</v>
       </c>
       <c r="J51" s="1">
-        <v>0.25</v>
+        <v>0.36</v>
       </c>
       <c r="K51" s="1">
-        <v>0.26</v>
+        <v>0.37</v>
       </c>
       <c r="L51" s="1">
-        <v>0.26</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D52" s="1">
-        <v>7.0000000000000007E-2</v>
+        <v>0.2</v>
       </c>
       <c r="E52" s="1">
-        <v>0.1</v>
+        <v>0.21</v>
       </c>
       <c r="F52" s="1">
-        <v>7.0000000000000007E-2</v>
+        <v>0.2</v>
       </c>
       <c r="G52" s="1">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="H52" s="1">
-        <v>7.0000000000000007E-2</v>
+        <v>0.2</v>
       </c>
       <c r="I52" s="1">
-        <v>0.08</v>
+        <v>0.21</v>
       </c>
       <c r="J52" s="1">
-        <v>7.0000000000000007E-2</v>
+        <v>0.2</v>
       </c>
       <c r="K52" s="1">
-        <v>7.0000000000000007E-2</v>
+        <v>0.2</v>
       </c>
       <c r="L52" s="1">
-        <v>0.1</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D53" s="1">
-        <v>7.0000000000000007E-2</v>
+        <v>0.25</v>
       </c>
       <c r="E53" s="1">
-        <v>0.1</v>
+        <v>0.26</v>
       </c>
       <c r="F53" s="1">
-        <v>7.0000000000000007E-2</v>
+        <v>0.25</v>
       </c>
       <c r="G53" s="1">
         <v>0</v>
       </c>
       <c r="H53" s="1">
-        <v>7.0000000000000007E-2</v>
+        <v>0.25</v>
       </c>
       <c r="I53" s="1">
-        <v>7.0000000000000007E-2</v>
+        <v>0.24</v>
       </c>
       <c r="J53" s="1">
-        <v>7.0000000000000007E-2</v>
+        <v>0.25</v>
       </c>
       <c r="K53" s="1">
-        <v>7.0000000000000007E-2</v>
+        <v>0.25</v>
       </c>
       <c r="L53" s="1">
-        <v>0.1</v>
+        <v>0.26</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D54" s="1">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="E54" s="1">
-        <v>0</v>
+        <v>0.26</v>
       </c>
       <c r="F54" s="1">
-        <v>0</v>
+        <v>0.26</v>
       </c>
       <c r="G54" s="1">
         <v>0</v>
       </c>
       <c r="H54" s="1">
-        <v>0</v>
+        <v>0.27</v>
       </c>
       <c r="I54" s="1">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="J54" s="1">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="K54" s="1">
-        <v>0</v>
+        <v>0.26</v>
       </c>
       <c r="L54" s="1">
-        <v>0</v>
+        <v>0.26</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.35">
@@ -3140,37 +3109,37 @@
         <v>20</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D55" s="1">
-        <v>0</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="E55" s="1">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="F55" s="1">
-        <v>0</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="G55" s="1">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="H55" s="1">
-        <v>0</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="I55" s="1">
-        <v>0</v>
+        <v>0.08</v>
       </c>
       <c r="J55" s="1">
-        <v>0</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="K55" s="1">
-        <v>0</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="L55" s="1">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.35">
@@ -3178,37 +3147,37 @@
         <v>20</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D56" s="1">
-        <v>0</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="E56" s="1">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="F56" s="1">
-        <v>0</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="G56" s="1">
         <v>0</v>
       </c>
       <c r="H56" s="1">
-        <v>0</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="I56" s="1">
-        <v>0</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="J56" s="1">
-        <v>0</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="K56" s="1">
-        <v>0</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="L56" s="1">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.35">
@@ -3216,10 +3185,10 @@
         <v>20</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D57" s="1">
         <v>0</v>
@@ -3251,116 +3220,116 @@
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D58" s="1">
-        <v>0.42</v>
+        <v>0</v>
       </c>
       <c r="E58" s="1">
-        <v>0.42</v>
+        <v>0</v>
       </c>
       <c r="F58" s="1">
-        <v>0.38</v>
+        <v>0</v>
       </c>
       <c r="G58" s="1">
-        <v>0.67</v>
+        <v>0</v>
       </c>
       <c r="H58" s="1">
-        <v>0.48</v>
+        <v>0</v>
       </c>
       <c r="I58" s="1">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="J58" s="1">
-        <v>0.63</v>
+        <v>0</v>
       </c>
       <c r="K58" s="1">
-        <v>0.38</v>
+        <v>0</v>
       </c>
       <c r="L58" s="1">
-        <v>0.4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D59" s="1">
-        <v>0.44</v>
+        <v>0</v>
       </c>
       <c r="E59" s="1">
-        <v>0.45</v>
+        <v>0</v>
       </c>
       <c r="F59" s="1">
-        <v>0.44</v>
+        <v>0</v>
       </c>
       <c r="G59" s="1">
         <v>0</v>
       </c>
       <c r="H59" s="1">
-        <v>0.48</v>
+        <v>0</v>
       </c>
       <c r="I59" s="1">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="J59" s="1">
-        <v>0.44</v>
+        <v>0</v>
       </c>
       <c r="K59" s="1">
-        <v>0.44</v>
+        <v>0</v>
       </c>
       <c r="L59" s="1">
-        <v>0.49</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D60" s="1">
-        <v>0.48</v>
+        <v>0</v>
       </c>
       <c r="E60" s="1">
-        <v>0.45</v>
+        <v>0</v>
       </c>
       <c r="F60" s="1">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="G60" s="1">
         <v>0</v>
       </c>
       <c r="H60" s="1">
-        <v>0.48</v>
+        <v>0</v>
       </c>
       <c r="I60" s="1">
-        <v>0.55000000000000004</v>
+        <v>0</v>
       </c>
       <c r="J60" s="1">
-        <v>0.48</v>
+        <v>0</v>
       </c>
       <c r="K60" s="1">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="L60" s="1">
-        <v>0.6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.35">
@@ -3368,37 +3337,37 @@
         <v>21</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D61" s="1">
-        <v>0.59</v>
+        <v>0.42</v>
       </c>
       <c r="E61" s="1">
-        <v>0.6</v>
+        <v>0.42</v>
       </c>
       <c r="F61" s="1">
-        <v>0.59</v>
+        <v>0.38</v>
       </c>
       <c r="G61" s="1">
-        <v>0</v>
+        <v>0.67</v>
       </c>
       <c r="H61" s="1">
-        <v>0.59</v>
+        <v>0.48</v>
       </c>
       <c r="I61" s="1">
-        <v>0.52</v>
+        <v>0.4</v>
       </c>
       <c r="J61" s="1">
-        <v>0.59</v>
+        <v>0.63</v>
       </c>
       <c r="K61" s="1">
-        <v>0.59</v>
+        <v>0.38</v>
       </c>
       <c r="L61" s="1">
-        <v>0.51</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.35">
@@ -3406,37 +3375,37 @@
         <v>21</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D62" s="1">
-        <v>0.54</v>
+        <v>0.44</v>
       </c>
       <c r="E62" s="1">
-        <v>0.63</v>
+        <v>0.45</v>
       </c>
       <c r="F62" s="1">
-        <v>0.54</v>
+        <v>0.44</v>
       </c>
       <c r="G62" s="1">
         <v>0</v>
       </c>
       <c r="H62" s="1">
-        <v>0.55000000000000004</v>
+        <v>0.48</v>
       </c>
       <c r="I62" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="J62" s="1">
+        <v>0.44</v>
+      </c>
+      <c r="K62" s="1">
+        <v>0.44</v>
+      </c>
+      <c r="L62" s="1">
         <v>0.49</v>
-      </c>
-      <c r="J62" s="1">
-        <v>0.49</v>
-      </c>
-      <c r="K62" s="1">
-        <v>0.54</v>
-      </c>
-      <c r="L62" s="1">
-        <v>0.5</v>
       </c>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.35">
@@ -3444,36 +3413,150 @@
         <v>21</v>
       </c>
       <c r="B63" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D63" s="1">
+        <v>0.48</v>
+      </c>
+      <c r="E63" s="1">
+        <v>0.45</v>
+      </c>
+      <c r="F63" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="G63" s="1">
+        <v>0</v>
+      </c>
+      <c r="H63" s="1">
+        <v>0.48</v>
+      </c>
+      <c r="I63" s="1">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="J63" s="1">
+        <v>0.48</v>
+      </c>
+      <c r="K63" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="L63" s="1">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A64" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D64" s="1">
+        <v>0.59</v>
+      </c>
+      <c r="E64" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="F64" s="1">
+        <v>0.59</v>
+      </c>
+      <c r="G64" s="1">
+        <v>0</v>
+      </c>
+      <c r="H64" s="1">
+        <v>0.59</v>
+      </c>
+      <c r="I64" s="1">
+        <v>0.52</v>
+      </c>
+      <c r="J64" s="1">
+        <v>0.59</v>
+      </c>
+      <c r="K64" s="1">
+        <v>0.59</v>
+      </c>
+      <c r="L64" s="1">
+        <v>0.51</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A65" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B65" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C63" s="1" t="s">
+      <c r="C65" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D65" s="1">
+        <v>0.54</v>
+      </c>
+      <c r="E65" s="1">
+        <v>0.63</v>
+      </c>
+      <c r="F65" s="1">
+        <v>0.54</v>
+      </c>
+      <c r="G65" s="1">
+        <v>0</v>
+      </c>
+      <c r="H65" s="1">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="I65" s="1">
+        <v>0.49</v>
+      </c>
+      <c r="J65" s="1">
+        <v>0.49</v>
+      </c>
+      <c r="K65" s="1">
+        <v>0.54</v>
+      </c>
+      <c r="L65" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A66" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C66" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D63" s="1">
+      <c r="D66" s="1">
         <v>0.54</v>
       </c>
-      <c r="E63" s="1">
+      <c r="E66" s="1">
         <v>0.5</v>
       </c>
-      <c r="F63" s="1">
+      <c r="F66" s="1">
         <v>0.54</v>
       </c>
-      <c r="G63" s="1">
+      <c r="G66" s="1">
         <v>0.4</v>
       </c>
-      <c r="H63" s="1">
+      <c r="H66" s="1">
         <v>0.54</v>
       </c>
-      <c r="I63" s="1">
+      <c r="I66" s="1">
         <v>0.56999999999999995</v>
       </c>
-      <c r="J63" s="1">
+      <c r="J66" s="1">
         <v>0.5</v>
       </c>
-      <c r="K63" s="1">
+      <c r="K66" s="1">
         <v>0.54</v>
       </c>
-      <c r="L63" s="1">
+      <c r="L66" s="1">
         <v>0.5</v>
       </c>
     </row>

</xml_diff>